<commit_message>
coverted to trees to radial and colored branches for report
</commit_message>
<xml_diff>
--- a/20 Results/datasets.xlsx
+++ b/20 Results/datasets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qx217\Documents\rotavirus\20 Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rotavirus\20 Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -105,7 +105,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,8 +118,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -127,16 +133,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -230,6 +288,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -265,6 +340,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -420,7 +512,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,584 +521,584 @@
     <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>1262</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>1485</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="5">
         <v>1582</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="4">
         <v>954</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="5">
         <v>1489</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>948</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="5">
         <v>2409</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <v>648</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="5">
         <v>1250</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="4">
         <v>642</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="5">
         <v>1668</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="4">
         <v>3288</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="5">
         <v>1584</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="4">
         <v>2760</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="5">
         <v>1661</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="4">
         <v>2319</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="5">
         <v>4937</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="5">
         <v>2646</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="5">
         <v>1913</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="4">
         <v>1206</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="5">
         <v>6586</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="4">
         <v>1107</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4">
         <v>28</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="4">
         <v>963</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="4">
         <v>46</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="4">
         <v>903</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="4">
         <v>18</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="4">
         <v>861</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="4">
         <v>28</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="4">
         <v>669</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="4">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="4">
         <v>47</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="4">
         <v>525</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="4">
         <v>19</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="4">
         <v>3480</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="4">
         <v>22</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="4">
         <v>2802</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="4">
         <v>17</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="4">
         <v>2289</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="4">
         <v>27</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="4">
         <v>2250</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="4">
         <v>94</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="4">
         <v>1173</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="4">
         <v>134</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="4">
         <v>753</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="4">
         <v>27</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="4">
         <v>1188</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="4">
         <v>27</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="4">
         <v>936</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="4">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="4">
         <v>28</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="4">
         <v>1206</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="4">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="4">
         <v>61</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="4">
         <v>450</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="4">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="4">
         <v>30</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="4">
         <v>531</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="4">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="4">
         <v>31</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="4">
         <v>3270</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" s="4">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="4">
         <v>35</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="4">
         <v>2658</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="4">
         <v>28</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="4">
         <v>2085</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="4">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="4">
         <v>76</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="4">
         <v>2244</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="4">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="4">
         <v>129</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="4">
         <v>1185</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" s="4">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="4">
         <v>227</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="4">
         <v>936</v>
       </c>
     </row>

</xml_diff>